<commit_message>
test finished, try semi supervise model
</commit_message>
<xml_diff>
--- a/data/Results.xlsx
+++ b/data/Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProject\spider\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6033DF90-9602-4508-A6E6-8CB748290D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D0EA1E-8DF9-4B9E-89F6-5BF0ED1C9D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40050" yWindow="1710" windowWidth="28800" windowHeight="11385" activeTab="1" xr2:uid="{111C6231-69C1-4C3E-BEA9-996E8DAA70A0}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{111C6231-69C1-4C3E-BEA9-996E8DAA70A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Danmaku" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="17">
   <si>
     <t>TextCNN</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1148,7 +1148,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:E13"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1565,8 +1565,23 @@
       <c r="E16">
         <v>95</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0.86539999999999995</v>
+      </c>
+      <c r="I16">
+        <v>0.94740000000000002</v>
+      </c>
+      <c r="J16">
+        <v>0.90449999999999997</v>
+      </c>
+      <c r="K16">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1582,8 +1597,23 @@
       <c r="E17">
         <v>105</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>0.94789999999999996</v>
+      </c>
+      <c r="I17">
+        <v>0.86670000000000003</v>
+      </c>
+      <c r="J17">
+        <v>0.90549999999999997</v>
+      </c>
+      <c r="K17">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1593,8 +1623,17 @@
       <c r="E18">
         <v>200</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="K18">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1610,8 +1649,23 @@
       <c r="E19">
         <v>200</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19">
+        <v>0.90669999999999995</v>
+      </c>
+      <c r="I19">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="J19">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="K19">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1627,8 +1681,23 @@
       <c r="E20">
         <v>200</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20">
+        <v>0.90869999999999995</v>
+      </c>
+      <c r="I20">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="J20">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="K20">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>12</v>
       </c>
@@ -1645,7 +1714,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>0</v>
       </c>
@@ -1662,7 +1731,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1679,7 +1748,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -1690,7 +1759,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -1707,7 +1776,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>5</v>
       </c>

</xml_diff>